<commit_message>
Template definition first draft.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_index_update_v5_4_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_index_update_v5_4_0.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="SampleTransfer" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Library" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Info" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Index" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
@@ -1700,7 +1700,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.21"/>
@@ -6534,7 +6534,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.33"/>
   </cols>
@@ -7501,7 +7501,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.5"/>

</xml_diff>

<commit_message>
Removed formula from template.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_index_update_v5_4_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_index_update_v5_4_0.xlsx
@@ -1266,10 +1266,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -1557,7 +1556,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1573,7 +1572,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1686,7 +1685,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.21"/>
@@ -1762,3840 +1761,2688 @@
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
-      <c r="E6" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C6))),C6,"")</f>
-        <v/>
-      </c>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C7))),C7,"")</f>
-        <v/>
-      </c>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C8))),C8,"")</f>
-        <v/>
-      </c>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C9))),C9,"")</f>
-        <v/>
-      </c>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C10))),C10,"")</f>
-        <v/>
-      </c>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C11))),C11,"")</f>
-        <v/>
-      </c>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C12))),C12,"")</f>
-        <v/>
-      </c>
+      <c r="E12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C13))),C13,"")</f>
-        <v/>
-      </c>
+      <c r="E13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C14))),C14,"")</f>
-        <v/>
-      </c>
+      <c r="E14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C15))),C15,"")</f>
-        <v/>
-      </c>
+      <c r="E15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C16))),C16,"")</f>
-        <v/>
-      </c>
+      <c r="E16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C17))),C17,"")</f>
-        <v/>
-      </c>
+      <c r="E17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C18))),C18,"")</f>
-        <v/>
-      </c>
+      <c r="E18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C19))),C19,"")</f>
-        <v/>
-      </c>
+      <c r="E19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C20))),C20,"")</f>
-        <v/>
-      </c>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C21))),C21,"")</f>
-        <v/>
-      </c>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C22))),C22,"")</f>
-        <v/>
-      </c>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C23))),C23,"")</f>
-        <v/>
-      </c>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="13"/>
-      <c r="E24" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C24))),C24,"")</f>
-        <v/>
-      </c>
+      <c r="E24" s="14"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="13"/>
-      <c r="E25" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C25))),C25,"")</f>
-        <v/>
-      </c>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C26))),C26,"")</f>
-        <v/>
-      </c>
+      <c r="E26" s="14"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="13"/>
-      <c r="E27" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C27))),C27,"")</f>
-        <v/>
-      </c>
+      <c r="E27" s="14"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C28))),C28,"")</f>
-        <v/>
-      </c>
+      <c r="E28" s="14"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="13"/>
-      <c r="E29" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C29))),C29,"")</f>
-        <v/>
-      </c>
+      <c r="E29" s="14"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
-      <c r="E30" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C30))),C30,"")</f>
-        <v/>
-      </c>
+      <c r="E30" s="14"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C31))),C31,"")</f>
-        <v/>
-      </c>
+      <c r="E31" s="14"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="13"/>
-      <c r="E32" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C32))),C32,"")</f>
-        <v/>
-      </c>
+      <c r="E32" s="14"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="11"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="13"/>
-      <c r="E33" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C33))),C33,"")</f>
-        <v/>
-      </c>
+      <c r="E33" s="14"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="11"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="13"/>
-      <c r="E34" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C34))),C34,"")</f>
-        <v/>
-      </c>
+      <c r="E34" s="14"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="11"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="13"/>
-      <c r="E35" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C35))),C35,"")</f>
-        <v/>
-      </c>
+      <c r="E35" s="14"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="11"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="13"/>
-      <c r="E36" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C36))),C36,"")</f>
-        <v/>
-      </c>
+      <c r="E36" s="14"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="11"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="13"/>
-      <c r="E37" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C37))),C37,"")</f>
-        <v/>
-      </c>
+      <c r="E37" s="14"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="11"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="13"/>
-      <c r="E38" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C38))),C38,"")</f>
-        <v/>
-      </c>
+      <c r="E38" s="14"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="11"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="13"/>
-      <c r="E39" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C39))),C39,"")</f>
-        <v/>
-      </c>
+      <c r="E39" s="14"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="11"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="13"/>
-      <c r="E40" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C40))),C40,"")</f>
-        <v/>
-      </c>
+      <c r="E40" s="14"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="11"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="13"/>
-      <c r="E41" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C41))),C41,"")</f>
-        <v/>
-      </c>
+      <c r="E41" s="14"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="11"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="13"/>
-      <c r="E42" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C42))),C42,"")</f>
-        <v/>
-      </c>
+      <c r="E42" s="14"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="11"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="13"/>
-      <c r="E43" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C43))),C43,"")</f>
-        <v/>
-      </c>
+      <c r="E43" s="14"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="11"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="13"/>
-      <c r="E44" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C44))),C44,"")</f>
-        <v/>
-      </c>
+      <c r="E44" s="14"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="11"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="13"/>
-      <c r="E45" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C45))),C45,"")</f>
-        <v/>
-      </c>
+      <c r="E45" s="14"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="11"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="13"/>
-      <c r="E46" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C46))),C46,"")</f>
-        <v/>
-      </c>
+      <c r="E46" s="14"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="11"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="13"/>
-      <c r="E47" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C47))),C47,"")</f>
-        <v/>
-      </c>
+      <c r="E47" s="14"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="11"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="13"/>
-      <c r="E48" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C48))),C48,"")</f>
-        <v/>
-      </c>
+      <c r="E48" s="14"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="11"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="13"/>
-      <c r="E49" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C49))),C49,"")</f>
-        <v/>
-      </c>
+      <c r="E49" s="14"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="11"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="13"/>
-      <c r="E50" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C50))),C50,"")</f>
-        <v/>
-      </c>
+      <c r="E50" s="14"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="11"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="13"/>
-      <c r="E51" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C51))),C51,"")</f>
-        <v/>
-      </c>
+      <c r="E51" s="14"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="11"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="13"/>
-      <c r="E52" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C52))),C52,"")</f>
-        <v/>
-      </c>
+      <c r="E52" s="14"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="11"/>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="13"/>
-      <c r="E53" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C53))),C53,"")</f>
-        <v/>
-      </c>
+      <c r="E53" s="14"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="11"/>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="13"/>
-      <c r="E54" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C54))),C54,"")</f>
-        <v/>
-      </c>
+      <c r="E54" s="14"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="11"/>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="13"/>
-      <c r="E55" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C55))),C55,"")</f>
-        <v/>
-      </c>
+      <c r="E55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="11"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="13"/>
-      <c r="E56" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C56))),C56,"")</f>
-        <v/>
-      </c>
+      <c r="E56" s="14"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="11"/>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="13"/>
-      <c r="E57" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C57))),C57,"")</f>
-        <v/>
-      </c>
+      <c r="E57" s="14"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="11"/>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="13"/>
-      <c r="E58" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C58))),C58,"")</f>
-        <v/>
-      </c>
+      <c r="E58" s="14"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="11"/>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="13"/>
-      <c r="E59" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C59))),C59,"")</f>
-        <v/>
-      </c>
+      <c r="E59" s="14"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="11"/>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="13"/>
-      <c r="E60" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C60))),C60,"")</f>
-        <v/>
-      </c>
+      <c r="E60" s="14"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="11"/>
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
-      <c r="E61" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C61))),C61,"")</f>
-        <v/>
-      </c>
+      <c r="E61" s="14"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="11"/>
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
-      <c r="E62" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C62))),C62,"")</f>
-        <v/>
-      </c>
+      <c r="E62" s="14"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="11"/>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
-      <c r="E63" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C63))),C63,"")</f>
-        <v/>
-      </c>
+      <c r="E63" s="14"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="11"/>
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
-      <c r="E64" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C64))),C64,"")</f>
-        <v/>
-      </c>
+      <c r="E64" s="14"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="11"/>
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
-      <c r="E65" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C65))),C65,"")</f>
-        <v/>
-      </c>
+      <c r="E65" s="14"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="11"/>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
-      <c r="E66" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C66))),C66,"")</f>
-        <v/>
-      </c>
+      <c r="E66" s="14"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="11"/>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
-      <c r="E67" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C67))),C67,"")</f>
-        <v/>
-      </c>
+      <c r="E67" s="14"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="11"/>
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
-      <c r="E68" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C68))),C68,"")</f>
-        <v/>
-      </c>
+      <c r="E68" s="14"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="11"/>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
-      <c r="E69" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C69))),C69,"")</f>
-        <v/>
-      </c>
+      <c r="E69" s="14"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="11"/>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
-      <c r="E70" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C70))),C70,"")</f>
-        <v/>
-      </c>
+      <c r="E70" s="14"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="11"/>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
-      <c r="E71" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C71))),C71,"")</f>
-        <v/>
-      </c>
+      <c r="E71" s="14"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="11"/>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
-      <c r="E72" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C72))),C72,"")</f>
-        <v/>
-      </c>
+      <c r="E72" s="14"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="11"/>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
-      <c r="E73" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C73))),C73,"")</f>
-        <v/>
-      </c>
+      <c r="E73" s="14"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="11"/>
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
-      <c r="E74" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C74))),C74,"")</f>
-        <v/>
-      </c>
+      <c r="E74" s="14"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="11"/>
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
-      <c r="E75" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C75))),C75,"")</f>
-        <v/>
-      </c>
+      <c r="E75" s="14"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="11"/>
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
-      <c r="E76" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C76))),C76,"")</f>
-        <v/>
-      </c>
+      <c r="E76" s="14"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="11"/>
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
-      <c r="E77" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C77))),C77,"")</f>
-        <v/>
-      </c>
+      <c r="E77" s="14"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="11"/>
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
-      <c r="E78" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C78))),C78,"")</f>
-        <v/>
-      </c>
+      <c r="E78" s="14"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="11"/>
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
-      <c r="E79" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C79))),C79,"")</f>
-        <v/>
-      </c>
+      <c r="E79" s="14"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="11"/>
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
-      <c r="E80" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C80))),C80,"")</f>
-        <v/>
-      </c>
+      <c r="E80" s="14"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="11"/>
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
-      <c r="E81" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C81))),C81,"")</f>
-        <v/>
-      </c>
+      <c r="E81" s="14"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="11"/>
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
-      <c r="E82" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C82))),C82,"")</f>
-        <v/>
-      </c>
+      <c r="E82" s="14"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="11"/>
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
-      <c r="E83" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C83))),C83,"")</f>
-        <v/>
-      </c>
+      <c r="E83" s="14"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="11"/>
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
-      <c r="E84" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C84))),C84,"")</f>
-        <v/>
-      </c>
+      <c r="E84" s="14"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="11"/>
       <c r="B85" s="12"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
-      <c r="E85" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C85))),C85,"")</f>
-        <v/>
-      </c>
+      <c r="E85" s="14"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="11"/>
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
-      <c r="E86" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C86))),C86,"")</f>
-        <v/>
-      </c>
+      <c r="E86" s="14"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="11"/>
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
-      <c r="E87" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C87))),C87,"")</f>
-        <v/>
-      </c>
+      <c r="E87" s="14"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="11"/>
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
-      <c r="E88" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C88))),C88,"")</f>
-        <v/>
-      </c>
+      <c r="E88" s="14"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="11"/>
       <c r="B89" s="12"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
-      <c r="E89" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C89))),C89,"")</f>
-        <v/>
-      </c>
+      <c r="E89" s="14"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="11"/>
       <c r="B90" s="12"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
-      <c r="E90" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C90))),C90,"")</f>
-        <v/>
-      </c>
+      <c r="E90" s="14"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="11"/>
       <c r="B91" s="12"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
-      <c r="E91" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C91))),C91,"")</f>
-        <v/>
-      </c>
+      <c r="E91" s="14"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="11"/>
       <c r="B92" s="12"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
-      <c r="E92" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C92))),C92,"")</f>
-        <v/>
-      </c>
+      <c r="E92" s="14"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="11"/>
       <c r="B93" s="12"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
-      <c r="E93" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C93))),C93,"")</f>
-        <v/>
-      </c>
+      <c r="E93" s="14"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="11"/>
       <c r="B94" s="12"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
-      <c r="E94" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C94))),C94,"")</f>
-        <v/>
-      </c>
+      <c r="E94" s="14"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="11"/>
       <c r="B95" s="12"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
-      <c r="E95" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C95))),C95,"")</f>
-        <v/>
-      </c>
+      <c r="E95" s="14"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="11"/>
       <c r="B96" s="12"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
-      <c r="E96" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C96))),C96,"")</f>
-        <v/>
-      </c>
+      <c r="E96" s="14"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="11"/>
       <c r="B97" s="12"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
-      <c r="E97" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C97))),C97,"")</f>
-        <v/>
-      </c>
+      <c r="E97" s="14"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="11"/>
       <c r="B98" s="12"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
-      <c r="E98" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C98))),C98,"")</f>
-        <v/>
-      </c>
+      <c r="E98" s="14"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="11"/>
       <c r="B99" s="12"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
-      <c r="E99" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C99))),C99,"")</f>
-        <v/>
-      </c>
+      <c r="E99" s="14"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="11"/>
       <c r="B100" s="12"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
-      <c r="E100" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C100))),C100,"")</f>
-        <v/>
-      </c>
+      <c r="E100" s="14"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="11"/>
       <c r="B101" s="12"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
-      <c r="E101" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C101))),C101,"")</f>
-        <v/>
-      </c>
+      <c r="E101" s="14"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="11"/>
       <c r="B102" s="12"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
-      <c r="E102" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C102))),C102,"")</f>
-        <v/>
-      </c>
+      <c r="E102" s="14"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="11"/>
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
-      <c r="E103" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C103))),C103,"")</f>
-        <v/>
-      </c>
+      <c r="E103" s="14"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="11"/>
       <c r="B104" s="12"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
-      <c r="E104" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C104))),C104,"")</f>
-        <v/>
-      </c>
+      <c r="E104" s="14"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="11"/>
       <c r="B105" s="12"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
-      <c r="E105" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C105))),C105,"")</f>
-        <v/>
-      </c>
+      <c r="E105" s="14"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="11"/>
       <c r="B106" s="12"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
-      <c r="E106" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C106))),C106,"")</f>
-        <v/>
-      </c>
+      <c r="E106" s="14"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="11"/>
       <c r="B107" s="12"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
-      <c r="E107" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C107))),C107,"")</f>
-        <v/>
-      </c>
+      <c r="E107" s="14"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="11"/>
       <c r="B108" s="12"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
-      <c r="E108" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C108))),C108,"")</f>
-        <v/>
-      </c>
+      <c r="E108" s="14"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="11"/>
       <c r="B109" s="12"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
-      <c r="E109" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C109))),C109,"")</f>
-        <v/>
-      </c>
+      <c r="E109" s="14"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="11"/>
       <c r="B110" s="12"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
-      <c r="E110" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C110))),C110,"")</f>
-        <v/>
-      </c>
+      <c r="E110" s="14"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="11"/>
       <c r="B111" s="12"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
-      <c r="E111" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C111))),C111,"")</f>
-        <v/>
-      </c>
+      <c r="E111" s="14"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="11"/>
       <c r="B112" s="12"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
-      <c r="E112" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C112))),C112,"")</f>
-        <v/>
-      </c>
+      <c r="E112" s="14"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="11"/>
       <c r="B113" s="12"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
-      <c r="E113" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C113))),C113,"")</f>
-        <v/>
-      </c>
+      <c r="E113" s="14"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="11"/>
       <c r="B114" s="12"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
-      <c r="E114" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C114))),C114,"")</f>
-        <v/>
-      </c>
+      <c r="E114" s="14"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="11"/>
       <c r="B115" s="12"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
-      <c r="E115" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C115))),C115,"")</f>
-        <v/>
-      </c>
+      <c r="E115" s="14"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="11"/>
       <c r="B116" s="12"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
-      <c r="E116" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C116))),C116,"")</f>
-        <v/>
-      </c>
+      <c r="E116" s="14"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="11"/>
       <c r="B117" s="12"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
-      <c r="E117" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C117))),C117,"")</f>
-        <v/>
-      </c>
+      <c r="E117" s="14"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="11"/>
       <c r="B118" s="12"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
-      <c r="E118" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C118))),C118,"")</f>
-        <v/>
-      </c>
+      <c r="E118" s="14"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="11"/>
       <c r="B119" s="12"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
-      <c r="E119" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C119))),C119,"")</f>
-        <v/>
-      </c>
+      <c r="E119" s="14"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="11"/>
       <c r="B120" s="12"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
-      <c r="E120" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C120))),C120,"")</f>
-        <v/>
-      </c>
+      <c r="E120" s="14"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="11"/>
       <c r="B121" s="12"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
-      <c r="E121" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C121))),C121,"")</f>
-        <v/>
-      </c>
+      <c r="E121" s="14"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="11"/>
       <c r="B122" s="12"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
-      <c r="E122" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C122))),C122,"")</f>
-        <v/>
-      </c>
+      <c r="E122" s="14"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="11"/>
       <c r="B123" s="12"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
-      <c r="E123" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C123))),C123,"")</f>
-        <v/>
-      </c>
+      <c r="E123" s="14"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="11"/>
       <c r="B124" s="12"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
-      <c r="E124" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C124))),C124,"")</f>
-        <v/>
-      </c>
+      <c r="E124" s="14"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="11"/>
       <c r="B125" s="12"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
-      <c r="E125" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C125))),C125,"")</f>
-        <v/>
-      </c>
+      <c r="E125" s="14"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="11"/>
       <c r="B126" s="12"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
-      <c r="E126" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C126))),C126,"")</f>
-        <v/>
-      </c>
+      <c r="E126" s="14"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="11"/>
       <c r="B127" s="12"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
-      <c r="E127" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C127))),C127,"")</f>
-        <v/>
-      </c>
+      <c r="E127" s="14"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="11"/>
       <c r="B128" s="12"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
-      <c r="E128" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C128))),C128,"")</f>
-        <v/>
-      </c>
+      <c r="E128" s="14"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="11"/>
       <c r="B129" s="12"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
-      <c r="E129" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C129))),C129,"")</f>
-        <v/>
-      </c>
+      <c r="E129" s="14"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="11"/>
       <c r="B130" s="12"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
-      <c r="E130" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C130))),C130,"")</f>
-        <v/>
-      </c>
+      <c r="E130" s="14"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="11"/>
       <c r="B131" s="12"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
-      <c r="E131" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C131))),C131,"")</f>
-        <v/>
-      </c>
+      <c r="E131" s="14"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="11"/>
       <c r="B132" s="12"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
-      <c r="E132" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C132))),C132,"")</f>
-        <v/>
-      </c>
+      <c r="E132" s="14"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="11"/>
       <c r="B133" s="12"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
-      <c r="E133" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C133))),C133,"")</f>
-        <v/>
-      </c>
+      <c r="E133" s="14"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="11"/>
       <c r="B134" s="12"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
-      <c r="E134" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C134))),C134,"")</f>
-        <v/>
-      </c>
+      <c r="E134" s="14"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="11"/>
       <c r="B135" s="12"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
-      <c r="E135" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C135))),C135,"")</f>
-        <v/>
-      </c>
+      <c r="E135" s="14"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="11"/>
       <c r="B136" s="12"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
-      <c r="E136" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C136))),C136,"")</f>
-        <v/>
-      </c>
+      <c r="E136" s="14"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="11"/>
       <c r="B137" s="12"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
-      <c r="E137" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C137))),C137,"")</f>
-        <v/>
-      </c>
+      <c r="E137" s="14"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="11"/>
       <c r="B138" s="12"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
-      <c r="E138" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C138))),C138,"")</f>
-        <v/>
-      </c>
+      <c r="E138" s="14"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="11"/>
       <c r="B139" s="12"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
-      <c r="E139" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C139))),C139,"")</f>
-        <v/>
-      </c>
+      <c r="E139" s="14"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="11"/>
       <c r="B140" s="12"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
-      <c r="E140" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C140))),C140,"")</f>
-        <v/>
-      </c>
+      <c r="E140" s="14"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="11"/>
       <c r="B141" s="12"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
-      <c r="E141" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C141))),C141,"")</f>
-        <v/>
-      </c>
+      <c r="E141" s="14"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="11"/>
       <c r="B142" s="12"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
-      <c r="E142" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C142))),C142,"")</f>
-        <v/>
-      </c>
+      <c r="E142" s="14"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="11"/>
       <c r="B143" s="12"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
-      <c r="E143" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C143))),C143,"")</f>
-        <v/>
-      </c>
+      <c r="E143" s="14"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="11"/>
       <c r="B144" s="12"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
-      <c r="E144" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C144))),C144,"")</f>
-        <v/>
-      </c>
+      <c r="E144" s="14"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="11"/>
       <c r="B145" s="12"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
-      <c r="E145" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C145))),C145,"")</f>
-        <v/>
-      </c>
+      <c r="E145" s="14"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="11"/>
       <c r="B146" s="12"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
-      <c r="E146" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C146))),C146,"")</f>
-        <v/>
-      </c>
+      <c r="E146" s="14"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="11"/>
       <c r="B147" s="12"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
-      <c r="E147" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C147))),C147,"")</f>
-        <v/>
-      </c>
+      <c r="E147" s="14"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="11"/>
       <c r="B148" s="12"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
-      <c r="E148" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C148))),C148,"")</f>
-        <v/>
-      </c>
+      <c r="E148" s="14"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="11"/>
       <c r="B149" s="12"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
-      <c r="E149" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C149))),C149,"")</f>
-        <v/>
-      </c>
+      <c r="E149" s="14"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="11"/>
       <c r="B150" s="12"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
-      <c r="E150" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C150))),C150,"")</f>
-        <v/>
-      </c>
+      <c r="E150" s="14"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="11"/>
       <c r="B151" s="12"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
-      <c r="E151" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C151))),C151,"")</f>
-        <v/>
-      </c>
+      <c r="E151" s="14"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="11"/>
       <c r="B152" s="12"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
-      <c r="E152" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C152))),C152,"")</f>
-        <v/>
-      </c>
+      <c r="E152" s="14"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="11"/>
       <c r="B153" s="12"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
-      <c r="E153" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C153))),C153,"")</f>
-        <v/>
-      </c>
+      <c r="E153" s="14"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="11"/>
       <c r="B154" s="12"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
-      <c r="E154" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C154))),C154,"")</f>
-        <v/>
-      </c>
+      <c r="E154" s="14"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="11"/>
       <c r="B155" s="12"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
-      <c r="E155" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C155))),C155,"")</f>
-        <v/>
-      </c>
+      <c r="E155" s="14"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="11"/>
       <c r="B156" s="12"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
-      <c r="E156" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C156))),C156,"")</f>
-        <v/>
-      </c>
+      <c r="E156" s="14"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="11"/>
       <c r="B157" s="12"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
-      <c r="E157" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C157))),C157,"")</f>
-        <v/>
-      </c>
+      <c r="E157" s="14"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="11"/>
       <c r="B158" s="12"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
-      <c r="E158" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C158))),C158,"")</f>
-        <v/>
-      </c>
+      <c r="E158" s="14"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="11"/>
       <c r="B159" s="12"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
-      <c r="E159" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C159))),C159,"")</f>
-        <v/>
-      </c>
+      <c r="E159" s="14"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="11"/>
       <c r="B160" s="12"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
-      <c r="E160" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C160))),C160,"")</f>
-        <v/>
-      </c>
+      <c r="E160" s="14"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="11"/>
       <c r="B161" s="12"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
-      <c r="E161" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C161))),C161,"")</f>
-        <v/>
-      </c>
+      <c r="E161" s="14"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="11"/>
       <c r="B162" s="12"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
-      <c r="E162" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C162))),C162,"")</f>
-        <v/>
-      </c>
+      <c r="E162" s="14"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="11"/>
       <c r="B163" s="12"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
-      <c r="E163" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C163))),C163,"")</f>
-        <v/>
-      </c>
+      <c r="E163" s="14"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="11"/>
       <c r="B164" s="12"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
-      <c r="E164" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C164))),C164,"")</f>
-        <v/>
-      </c>
+      <c r="E164" s="14"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="11"/>
       <c r="B165" s="12"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
-      <c r="E165" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C165))),C165,"")</f>
-        <v/>
-      </c>
+      <c r="E165" s="14"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="11"/>
       <c r="B166" s="12"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
-      <c r="E166" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C166))),C166,"")</f>
-        <v/>
-      </c>
+      <c r="E166" s="14"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="11"/>
       <c r="B167" s="12"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
-      <c r="E167" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C167))),C167,"")</f>
-        <v/>
-      </c>
+      <c r="E167" s="14"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="11"/>
       <c r="B168" s="12"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
-      <c r="E168" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C168))),C168,"")</f>
-        <v/>
-      </c>
+      <c r="E168" s="14"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="11"/>
       <c r="B169" s="12"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
-      <c r="E169" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C169))),C169,"")</f>
-        <v/>
-      </c>
+      <c r="E169" s="14"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="11"/>
       <c r="B170" s="12"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
-      <c r="E170" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C170))),C170,"")</f>
-        <v/>
-      </c>
+      <c r="E170" s="14"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="11"/>
       <c r="B171" s="12"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
-      <c r="E171" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C171))),C171,"")</f>
-        <v/>
-      </c>
+      <c r="E171" s="14"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="11"/>
       <c r="B172" s="12"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
-      <c r="E172" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C172))),C172,"")</f>
-        <v/>
-      </c>
+      <c r="E172" s="14"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="11"/>
       <c r="B173" s="12"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
-      <c r="E173" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C173))),C173,"")</f>
-        <v/>
-      </c>
+      <c r="E173" s="14"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="11"/>
       <c r="B174" s="12"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
-      <c r="E174" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C174))),C174,"")</f>
-        <v/>
-      </c>
+      <c r="E174" s="14"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="11"/>
       <c r="B175" s="12"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
-      <c r="E175" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C175))),C175,"")</f>
-        <v/>
-      </c>
+      <c r="E175" s="14"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="11"/>
       <c r="B176" s="12"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
-      <c r="E176" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C176))),C176,"")</f>
-        <v/>
-      </c>
+      <c r="E176" s="14"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="11"/>
       <c r="B177" s="12"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
-      <c r="E177" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C177))),C177,"")</f>
-        <v/>
-      </c>
+      <c r="E177" s="14"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="11"/>
       <c r="B178" s="12"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
-      <c r="E178" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C178))),C178,"")</f>
-        <v/>
-      </c>
+      <c r="E178" s="14"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="11"/>
       <c r="B179" s="12"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
-      <c r="E179" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C179))),C179,"")</f>
-        <v/>
-      </c>
+      <c r="E179" s="14"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="11"/>
       <c r="B180" s="12"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
-      <c r="E180" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C180))),C180,"")</f>
-        <v/>
-      </c>
+      <c r="E180" s="14"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="11"/>
       <c r="B181" s="12"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
-      <c r="E181" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C181))),C181,"")</f>
-        <v/>
-      </c>
+      <c r="E181" s="14"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="11"/>
       <c r="B182" s="12"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
-      <c r="E182" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C182))),C182,"")</f>
-        <v/>
-      </c>
+      <c r="E182" s="14"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="11"/>
       <c r="B183" s="12"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
-      <c r="E183" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C183))),C183,"")</f>
-        <v/>
-      </c>
+      <c r="E183" s="14"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="11"/>
       <c r="B184" s="12"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
-      <c r="E184" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C184))),C184,"")</f>
-        <v/>
-      </c>
+      <c r="E184" s="14"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="11"/>
       <c r="B185" s="12"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
-      <c r="E185" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C185))),C185,"")</f>
-        <v/>
-      </c>
+      <c r="E185" s="14"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="11"/>
       <c r="B186" s="12"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
-      <c r="E186" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C186))),C186,"")</f>
-        <v/>
-      </c>
+      <c r="E186" s="14"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="11"/>
       <c r="B187" s="12"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
-      <c r="E187" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C187))),C187,"")</f>
-        <v/>
-      </c>
+      <c r="E187" s="14"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="11"/>
       <c r="B188" s="12"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
-      <c r="E188" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C188))),C188,"")</f>
-        <v/>
-      </c>
+      <c r="E188" s="14"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="11"/>
       <c r="B189" s="12"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
-      <c r="E189" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C189))),C189,"")</f>
-        <v/>
-      </c>
+      <c r="E189" s="14"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="11"/>
       <c r="B190" s="12"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
-      <c r="E190" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C190))),C190,"")</f>
-        <v/>
-      </c>
+      <c r="E190" s="14"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="11"/>
       <c r="B191" s="12"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
-      <c r="E191" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C191))),C191,"")</f>
-        <v/>
-      </c>
+      <c r="E191" s="14"/>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="11"/>
       <c r="B192" s="12"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
-      <c r="E192" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C192))),C192,"")</f>
-        <v/>
-      </c>
+      <c r="E192" s="14"/>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="11"/>
       <c r="B193" s="12"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
-      <c r="E193" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C193))),C193,"")</f>
-        <v/>
-      </c>
+      <c r="E193" s="14"/>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="11"/>
       <c r="B194" s="12"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
-      <c r="E194" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C194))),C194,"")</f>
-        <v/>
-      </c>
+      <c r="E194" s="14"/>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="11"/>
       <c r="B195" s="12"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
-      <c r="E195" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C195))),C195,"")</f>
-        <v/>
-      </c>
+      <c r="E195" s="14"/>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="11"/>
       <c r="B196" s="12"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
-      <c r="E196" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C196))),C196,"")</f>
-        <v/>
-      </c>
+      <c r="E196" s="14"/>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="11"/>
       <c r="B197" s="12"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
-      <c r="E197" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C197))),C197,"")</f>
-        <v/>
-      </c>
+      <c r="E197" s="14"/>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="11"/>
       <c r="B198" s="12"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
-      <c r="E198" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C198))),C198,"")</f>
-        <v/>
-      </c>
+      <c r="E198" s="14"/>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="11"/>
       <c r="B199" s="12"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
-      <c r="E199" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C199))),C199,"")</f>
-        <v/>
-      </c>
+      <c r="E199" s="14"/>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="11"/>
       <c r="B200" s="12"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
-      <c r="E200" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C200))),C200,"")</f>
-        <v/>
-      </c>
+      <c r="E200" s="14"/>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="11"/>
       <c r="B201" s="12"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
-      <c r="E201" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C201))),C201,"")</f>
-        <v/>
-      </c>
+      <c r="E201" s="14"/>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="11"/>
       <c r="B202" s="12"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
-      <c r="E202" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C202))),C202,"")</f>
-        <v/>
-      </c>
+      <c r="E202" s="14"/>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="11"/>
       <c r="B203" s="12"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
-      <c r="E203" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C203))),C203,"")</f>
-        <v/>
-      </c>
+      <c r="E203" s="14"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="11"/>
       <c r="B204" s="12"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
-      <c r="E204" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C204))),C204,"")</f>
-        <v/>
-      </c>
+      <c r="E204" s="14"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="11"/>
       <c r="B205" s="12"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
-      <c r="E205" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C205))),C205,"")</f>
-        <v/>
-      </c>
+      <c r="E205" s="14"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="11"/>
       <c r="B206" s="12"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
-      <c r="E206" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C206))),C206,"")</f>
-        <v/>
-      </c>
+      <c r="E206" s="14"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="11"/>
       <c r="B207" s="12"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
-      <c r="E207" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C207))),C207,"")</f>
-        <v/>
-      </c>
+      <c r="E207" s="14"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="11"/>
       <c r="B208" s="12"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
-      <c r="E208" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C208))),C208,"")</f>
-        <v/>
-      </c>
+      <c r="E208" s="14"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="11"/>
       <c r="B209" s="12"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
-      <c r="E209" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C209))),C209,"")</f>
-        <v/>
-      </c>
+      <c r="E209" s="14"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="11"/>
       <c r="B210" s="12"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
-      <c r="E210" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C210))),C210,"")</f>
-        <v/>
-      </c>
+      <c r="E210" s="14"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="11"/>
       <c r="B211" s="12"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
-      <c r="E211" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C211))),C211,"")</f>
-        <v/>
-      </c>
+      <c r="E211" s="14"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="11"/>
       <c r="B212" s="12"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
-      <c r="E212" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C212))),C212,"")</f>
-        <v/>
-      </c>
+      <c r="E212" s="14"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="11"/>
       <c r="B213" s="12"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
-      <c r="E213" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C213))),C213,"")</f>
-        <v/>
-      </c>
+      <c r="E213" s="14"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="11"/>
       <c r="B214" s="12"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
-      <c r="E214" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C214))),C214,"")</f>
-        <v/>
-      </c>
+      <c r="E214" s="14"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="11"/>
       <c r="B215" s="12"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
-      <c r="E215" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C215))),C215,"")</f>
-        <v/>
-      </c>
+      <c r="E215" s="14"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="11"/>
       <c r="B216" s="12"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
-      <c r="E216" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C216))),C216,"")</f>
-        <v/>
-      </c>
+      <c r="E216" s="14"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="11"/>
       <c r="B217" s="12"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
-      <c r="E217" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C217))),C217,"")</f>
-        <v/>
-      </c>
+      <c r="E217" s="14"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="11"/>
       <c r="B218" s="12"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
-      <c r="E218" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C218))),C218,"")</f>
-        <v/>
-      </c>
+      <c r="E218" s="14"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="11"/>
       <c r="B219" s="12"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
-      <c r="E219" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C219))),C219,"")</f>
-        <v/>
-      </c>
+      <c r="E219" s="14"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="11"/>
       <c r="B220" s="12"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
-      <c r="E220" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C220))),C220,"")</f>
-        <v/>
-      </c>
+      <c r="E220" s="14"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="11"/>
       <c r="B221" s="12"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
-      <c r="E221" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C221))),C221,"")</f>
-        <v/>
-      </c>
+      <c r="E221" s="14"/>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="11"/>
       <c r="B222" s="12"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
-      <c r="E222" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C222))),C222,"")</f>
-        <v/>
-      </c>
+      <c r="E222" s="14"/>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="11"/>
       <c r="B223" s="12"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
-      <c r="E223" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C223))),C223,"")</f>
-        <v/>
-      </c>
+      <c r="E223" s="14"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="11"/>
       <c r="B224" s="12"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
-      <c r="E224" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C224))),C224,"")</f>
-        <v/>
-      </c>
+      <c r="E224" s="14"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="11"/>
       <c r="B225" s="12"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
-      <c r="E225" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C225))),C225,"")</f>
-        <v/>
-      </c>
+      <c r="E225" s="14"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="11"/>
       <c r="B226" s="12"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
-      <c r="E226" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C226))),C226,"")</f>
-        <v/>
-      </c>
+      <c r="E226" s="14"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="11"/>
       <c r="B227" s="12"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
-      <c r="E227" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C227))),C227,"")</f>
-        <v/>
-      </c>
+      <c r="E227" s="14"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="11"/>
       <c r="B228" s="12"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
-      <c r="E228" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C228))),C228,"")</f>
-        <v/>
-      </c>
+      <c r="E228" s="14"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="11"/>
       <c r="B229" s="12"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
-      <c r="E229" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C229))),C229,"")</f>
-        <v/>
-      </c>
+      <c r="E229" s="14"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="11"/>
       <c r="B230" s="12"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
-      <c r="E230" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C230))),C230,"")</f>
-        <v/>
-      </c>
+      <c r="E230" s="14"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="11"/>
       <c r="B231" s="12"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
-      <c r="E231" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C231))),C231,"")</f>
-        <v/>
-      </c>
+      <c r="E231" s="14"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="11"/>
       <c r="B232" s="12"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
-      <c r="E232" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C232))),C232,"")</f>
-        <v/>
-      </c>
+      <c r="E232" s="14"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="11"/>
       <c r="B233" s="12"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
-      <c r="E233" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C233))),C233,"")</f>
-        <v/>
-      </c>
+      <c r="E233" s="14"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="11"/>
       <c r="B234" s="12"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
-      <c r="E234" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C234))),C234,"")</f>
-        <v/>
-      </c>
+      <c r="E234" s="14"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="11"/>
       <c r="B235" s="12"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
-      <c r="E235" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C235))),C235,"")</f>
-        <v/>
-      </c>
+      <c r="E235" s="14"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="11"/>
       <c r="B236" s="12"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
-      <c r="E236" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C236))),C236,"")</f>
-        <v/>
-      </c>
+      <c r="E236" s="14"/>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="11"/>
       <c r="B237" s="12"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
-      <c r="E237" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C237))),C237,"")</f>
-        <v/>
-      </c>
+      <c r="E237" s="14"/>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="11"/>
       <c r="B238" s="12"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
-      <c r="E238" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C238))),C238,"")</f>
-        <v/>
-      </c>
+      <c r="E238" s="14"/>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="11"/>
       <c r="B239" s="12"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
-      <c r="E239" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C239))),C239,"")</f>
-        <v/>
-      </c>
+      <c r="E239" s="14"/>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="11"/>
       <c r="B240" s="12"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
-      <c r="E240" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C240))),C240,"")</f>
-        <v/>
-      </c>
+      <c r="E240" s="14"/>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="11"/>
       <c r="B241" s="12"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
-      <c r="E241" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C241))),C241,"")</f>
-        <v/>
-      </c>
+      <c r="E241" s="14"/>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="11"/>
       <c r="B242" s="12"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
-      <c r="E242" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C242))),C242,"")</f>
-        <v/>
-      </c>
+      <c r="E242" s="14"/>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="11"/>
       <c r="B243" s="12"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
-      <c r="E243" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C243))),C243,"")</f>
-        <v/>
-      </c>
+      <c r="E243" s="14"/>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="11"/>
       <c r="B244" s="12"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
-      <c r="E244" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C244))),C244,"")</f>
-        <v/>
-      </c>
+      <c r="E244" s="14"/>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="11"/>
       <c r="B245" s="12"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
-      <c r="E245" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C245))),C245,"")</f>
-        <v/>
-      </c>
+      <c r="E245" s="14"/>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="11"/>
       <c r="B246" s="12"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
-      <c r="E246" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C246))),C246,"")</f>
-        <v/>
-      </c>
+      <c r="E246" s="14"/>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="11"/>
       <c r="B247" s="12"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
-      <c r="E247" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C247))),C247,"")</f>
-        <v/>
-      </c>
+      <c r="E247" s="14"/>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="11"/>
       <c r="B248" s="12"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
-      <c r="E248" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C248))),C248,"")</f>
-        <v/>
-      </c>
+      <c r="E248" s="14"/>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="11"/>
       <c r="B249" s="12"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
-      <c r="E249" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C249))),C249,"")</f>
-        <v/>
-      </c>
+      <c r="E249" s="14"/>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="11"/>
       <c r="B250" s="12"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
-      <c r="E250" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C250))),C250,"")</f>
-        <v/>
-      </c>
+      <c r="E250" s="14"/>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="11"/>
       <c r="B251" s="12"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
-      <c r="E251" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C251))),C251,"")</f>
-        <v/>
-      </c>
+      <c r="E251" s="14"/>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="11"/>
       <c r="B252" s="12"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
-      <c r="E252" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C252))),C252,"")</f>
-        <v/>
-      </c>
+      <c r="E252" s="14"/>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="11"/>
       <c r="B253" s="12"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
-      <c r="E253" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C253))),C253,"")</f>
-        <v/>
-      </c>
+      <c r="E253" s="14"/>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="11"/>
       <c r="B254" s="12"/>
       <c r="C254" s="12"/>
       <c r="D254" s="13"/>
-      <c r="E254" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C254))),C254,"")</f>
-        <v/>
-      </c>
+      <c r="E254" s="14"/>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="11"/>
       <c r="B255" s="12"/>
       <c r="C255" s="12"/>
       <c r="D255" s="13"/>
-      <c r="E255" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C255))),C255,"")</f>
-        <v/>
-      </c>
+      <c r="E255" s="14"/>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="11"/>
       <c r="B256" s="12"/>
       <c r="C256" s="12"/>
       <c r="D256" s="13"/>
-      <c r="E256" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C256))),C256,"")</f>
-        <v/>
-      </c>
+      <c r="E256" s="14"/>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A257" s="11"/>
       <c r="B257" s="12"/>
       <c r="C257" s="12"/>
       <c r="D257" s="13"/>
-      <c r="E257" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C257))),C257,"")</f>
-        <v/>
-      </c>
+      <c r="E257" s="14"/>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A258" s="11"/>
       <c r="B258" s="12"/>
       <c r="C258" s="12"/>
       <c r="D258" s="13"/>
-      <c r="E258" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C258))),C258,"")</f>
-        <v/>
-      </c>
+      <c r="E258" s="14"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A259" s="11"/>
       <c r="B259" s="12"/>
       <c r="C259" s="12"/>
       <c r="D259" s="13"/>
-      <c r="E259" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C259))),C259,"")</f>
-        <v/>
-      </c>
+      <c r="E259" s="14"/>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A260" s="11"/>
       <c r="B260" s="12"/>
       <c r="C260" s="12"/>
       <c r="D260" s="13"/>
-      <c r="E260" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C260))),C260,"")</f>
-        <v/>
-      </c>
+      <c r="E260" s="14"/>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A261" s="11"/>
       <c r="B261" s="12"/>
       <c r="C261" s="12"/>
       <c r="D261" s="13"/>
-      <c r="E261" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C261))),C261,"")</f>
-        <v/>
-      </c>
+      <c r="E261" s="14"/>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A262" s="11"/>
       <c r="B262" s="12"/>
       <c r="C262" s="12"/>
       <c r="D262" s="13"/>
-      <c r="E262" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C262))),C262,"")</f>
-        <v/>
-      </c>
+      <c r="E262" s="14"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A263" s="11"/>
       <c r="B263" s="12"/>
       <c r="C263" s="12"/>
       <c r="D263" s="13"/>
-      <c r="E263" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C263))),C263,"")</f>
-        <v/>
-      </c>
+      <c r="E263" s="14"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A264" s="11"/>
       <c r="B264" s="12"/>
       <c r="C264" s="12"/>
       <c r="D264" s="13"/>
-      <c r="E264" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C264))),C264,"")</f>
-        <v/>
-      </c>
+      <c r="E264" s="14"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A265" s="11"/>
       <c r="B265" s="12"/>
       <c r="C265" s="12"/>
       <c r="D265" s="13"/>
-      <c r="E265" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C265))),C265,"")</f>
-        <v/>
-      </c>
+      <c r="E265" s="14"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A266" s="11"/>
       <c r="B266" s="12"/>
       <c r="C266" s="12"/>
       <c r="D266" s="13"/>
-      <c r="E266" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C266))),C266,"")</f>
-        <v/>
-      </c>
+      <c r="E266" s="14"/>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A267" s="11"/>
       <c r="B267" s="12"/>
       <c r="C267" s="12"/>
       <c r="D267" s="13"/>
-      <c r="E267" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C267))),C267,"")</f>
-        <v/>
-      </c>
+      <c r="E267" s="14"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A268" s="11"/>
       <c r="B268" s="12"/>
       <c r="C268" s="12"/>
       <c r="D268" s="13"/>
-      <c r="E268" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C268))),C268,"")</f>
-        <v/>
-      </c>
+      <c r="E268" s="14"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A269" s="11"/>
       <c r="B269" s="12"/>
       <c r="C269" s="12"/>
       <c r="D269" s="13"/>
-      <c r="E269" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C269))),C269,"")</f>
-        <v/>
-      </c>
+      <c r="E269" s="14"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A270" s="11"/>
       <c r="B270" s="12"/>
       <c r="C270" s="12"/>
       <c r="D270" s="13"/>
-      <c r="E270" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C270))),C270,"")</f>
-        <v/>
-      </c>
+      <c r="E270" s="14"/>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A271" s="11"/>
       <c r="B271" s="12"/>
       <c r="C271" s="12"/>
       <c r="D271" s="13"/>
-      <c r="E271" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C271))),C271,"")</f>
-        <v/>
-      </c>
+      <c r="E271" s="14"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A272" s="11"/>
       <c r="B272" s="12"/>
       <c r="C272" s="12"/>
       <c r="D272" s="13"/>
-      <c r="E272" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C272))),C272,"")</f>
-        <v/>
-      </c>
+      <c r="E272" s="14"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A273" s="11"/>
       <c r="B273" s="12"/>
       <c r="C273" s="12"/>
       <c r="D273" s="13"/>
-      <c r="E273" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C273))),C273,"")</f>
-        <v/>
-      </c>
+      <c r="E273" s="14"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="11"/>
       <c r="B274" s="12"/>
       <c r="C274" s="12"/>
       <c r="D274" s="13"/>
-      <c r="E274" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C274))),C274,"")</f>
-        <v/>
-      </c>
+      <c r="E274" s="14"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A275" s="11"/>
       <c r="B275" s="12"/>
       <c r="C275" s="12"/>
       <c r="D275" s="13"/>
-      <c r="E275" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C275))),C275,"")</f>
-        <v/>
-      </c>
+      <c r="E275" s="14"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A276" s="11"/>
       <c r="B276" s="12"/>
       <c r="C276" s="12"/>
       <c r="D276" s="13"/>
-      <c r="E276" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C276))),C276,"")</f>
-        <v/>
-      </c>
+      <c r="E276" s="14"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="11"/>
       <c r="B277" s="12"/>
       <c r="C277" s="12"/>
       <c r="D277" s="13"/>
-      <c r="E277" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C277))),C277,"")</f>
-        <v/>
-      </c>
+      <c r="E277" s="14"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A278" s="11"/>
       <c r="B278" s="12"/>
       <c r="C278" s="12"/>
       <c r="D278" s="13"/>
-      <c r="E278" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C278))),C278,"")</f>
-        <v/>
-      </c>
+      <c r="E278" s="14"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A279" s="11"/>
       <c r="B279" s="12"/>
       <c r="C279" s="12"/>
       <c r="D279" s="13"/>
-      <c r="E279" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C279))),C279,"")</f>
-        <v/>
-      </c>
+      <c r="E279" s="14"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A280" s="11"/>
       <c r="B280" s="12"/>
       <c r="C280" s="12"/>
       <c r="D280" s="13"/>
-      <c r="E280" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C280))),C280,"")</f>
-        <v/>
-      </c>
+      <c r="E280" s="14"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A281" s="11"/>
       <c r="B281" s="12"/>
       <c r="C281" s="12"/>
       <c r="D281" s="13"/>
-      <c r="E281" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C281))),C281,"")</f>
-        <v/>
-      </c>
+      <c r="E281" s="14"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A282" s="11"/>
       <c r="B282" s="12"/>
       <c r="C282" s="12"/>
       <c r="D282" s="13"/>
-      <c r="E282" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C282))),C282,"")</f>
-        <v/>
-      </c>
+      <c r="E282" s="14"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A283" s="11"/>
       <c r="B283" s="12"/>
       <c r="C283" s="12"/>
       <c r="D283" s="13"/>
-      <c r="E283" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C283))),C283,"")</f>
-        <v/>
-      </c>
+      <c r="E283" s="14"/>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="11"/>
       <c r="B284" s="12"/>
       <c r="C284" s="12"/>
       <c r="D284" s="13"/>
-      <c r="E284" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C284))),C284,"")</f>
-        <v/>
-      </c>
+      <c r="E284" s="14"/>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="11"/>
       <c r="B285" s="12"/>
       <c r="C285" s="12"/>
       <c r="D285" s="13"/>
-      <c r="E285" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C285))),C285,"")</f>
-        <v/>
-      </c>
+      <c r="E285" s="14"/>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="11"/>
       <c r="B286" s="12"/>
       <c r="C286" s="12"/>
       <c r="D286" s="13"/>
-      <c r="E286" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C286))),C286,"")</f>
-        <v/>
-      </c>
+      <c r="E286" s="14"/>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="11"/>
       <c r="B287" s="12"/>
       <c r="C287" s="12"/>
       <c r="D287" s="13"/>
-      <c r="E287" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C287))),C287,"")</f>
-        <v/>
-      </c>
+      <c r="E287" s="14"/>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="11"/>
       <c r="B288" s="12"/>
       <c r="C288" s="12"/>
       <c r="D288" s="13"/>
-      <c r="E288" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C288))),C288,"")</f>
-        <v/>
-      </c>
+      <c r="E288" s="14"/>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="11"/>
       <c r="B289" s="12"/>
       <c r="C289" s="12"/>
       <c r="D289" s="13"/>
-      <c r="E289" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C289))),C289,"")</f>
-        <v/>
-      </c>
+      <c r="E289" s="14"/>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="11"/>
       <c r="B290" s="12"/>
       <c r="C290" s="12"/>
       <c r="D290" s="13"/>
-      <c r="E290" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C290))),C290,"")</f>
-        <v/>
-      </c>
+      <c r="E290" s="14"/>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="11"/>
       <c r="B291" s="12"/>
       <c r="C291" s="12"/>
       <c r="D291" s="13"/>
-      <c r="E291" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C291))),C291,"")</f>
-        <v/>
-      </c>
+      <c r="E291" s="14"/>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="11"/>
       <c r="B292" s="12"/>
       <c r="C292" s="12"/>
       <c r="D292" s="13"/>
-      <c r="E292" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C292))),C292,"")</f>
-        <v/>
-      </c>
+      <c r="E292" s="14"/>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="11"/>
       <c r="B293" s="12"/>
       <c r="C293" s="12"/>
       <c r="D293" s="13"/>
-      <c r="E293" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C293))),C293,"")</f>
-        <v/>
-      </c>
+      <c r="E293" s="14"/>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="11"/>
       <c r="B294" s="12"/>
       <c r="C294" s="12"/>
       <c r="D294" s="13"/>
-      <c r="E294" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C294))),C294,"")</f>
-        <v/>
-      </c>
+      <c r="E294" s="14"/>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="11"/>
       <c r="B295" s="12"/>
       <c r="C295" s="12"/>
       <c r="D295" s="13"/>
-      <c r="E295" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C295))),C295,"")</f>
-        <v/>
-      </c>
+      <c r="E295" s="14"/>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A296" s="11"/>
       <c r="B296" s="12"/>
       <c r="C296" s="12"/>
       <c r="D296" s="13"/>
-      <c r="E296" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C296))),C296,"")</f>
-        <v/>
-      </c>
+      <c r="E296" s="14"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A297" s="11"/>
       <c r="B297" s="12"/>
       <c r="C297" s="12"/>
       <c r="D297" s="13"/>
-      <c r="E297" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C297))),C297,"")</f>
-        <v/>
-      </c>
+      <c r="E297" s="14"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A298" s="11"/>
       <c r="B298" s="12"/>
       <c r="C298" s="12"/>
       <c r="D298" s="13"/>
-      <c r="E298" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C298))),C298,"")</f>
-        <v/>
-      </c>
+      <c r="E298" s="14"/>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A299" s="11"/>
       <c r="B299" s="12"/>
       <c r="C299" s="12"/>
       <c r="D299" s="13"/>
-      <c r="E299" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C299))),C299,"")</f>
-        <v/>
-      </c>
+      <c r="E299" s="14"/>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="11"/>
       <c r="B300" s="12"/>
       <c r="C300" s="12"/>
       <c r="D300" s="13"/>
-      <c r="E300" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C300))),C300,"")</f>
-        <v/>
-      </c>
+      <c r="E300" s="14"/>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="11"/>
       <c r="B301" s="12"/>
       <c r="C301" s="12"/>
       <c r="D301" s="13"/>
-      <c r="E301" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C301))),C301,"")</f>
-        <v/>
-      </c>
+      <c r="E301" s="14"/>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A302" s="11"/>
       <c r="B302" s="12"/>
       <c r="C302" s="12"/>
       <c r="D302" s="13"/>
-      <c r="E302" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C302))),C302,"")</f>
-        <v/>
-      </c>
+      <c r="E302" s="14"/>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="11"/>
       <c r="B303" s="12"/>
       <c r="C303" s="12"/>
       <c r="D303" s="13"/>
-      <c r="E303" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C303))),C303,"")</f>
-        <v/>
-      </c>
+      <c r="E303" s="14"/>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A304" s="11"/>
       <c r="B304" s="12"/>
       <c r="C304" s="12"/>
       <c r="D304" s="13"/>
-      <c r="E304" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C304))),C304,"")</f>
-        <v/>
-      </c>
+      <c r="E304" s="14"/>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A305" s="11"/>
       <c r="B305" s="12"/>
       <c r="C305" s="12"/>
       <c r="D305" s="13"/>
-      <c r="E305" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C305))),C305,"")</f>
-        <v/>
-      </c>
+      <c r="E305" s="14"/>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A306" s="11"/>
       <c r="B306" s="12"/>
       <c r="C306" s="12"/>
       <c r="D306" s="13"/>
-      <c r="E306" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C306))),C306,"")</f>
-        <v/>
-      </c>
+      <c r="E306" s="14"/>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A307" s="11"/>
       <c r="B307" s="12"/>
       <c r="C307" s="12"/>
       <c r="D307" s="13"/>
-      <c r="E307" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C307))),C307,"")</f>
-        <v/>
-      </c>
+      <c r="E307" s="14"/>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A308" s="11"/>
       <c r="B308" s="12"/>
       <c r="C308" s="12"/>
       <c r="D308" s="13"/>
-      <c r="E308" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C308))),C308,"")</f>
-        <v/>
-      </c>
+      <c r="E308" s="14"/>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A309" s="11"/>
       <c r="B309" s="12"/>
       <c r="C309" s="12"/>
       <c r="D309" s="13"/>
-      <c r="E309" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C309))),C309,"")</f>
-        <v/>
-      </c>
+      <c r="E309" s="14"/>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A310" s="11"/>
       <c r="B310" s="12"/>
       <c r="C310" s="12"/>
       <c r="D310" s="13"/>
-      <c r="E310" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C310))),C310,"")</f>
-        <v/>
-      </c>
+      <c r="E310" s="14"/>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A311" s="11"/>
       <c r="B311" s="12"/>
       <c r="C311" s="12"/>
       <c r="D311" s="13"/>
-      <c r="E311" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C311))),C311,"")</f>
-        <v/>
-      </c>
+      <c r="E311" s="14"/>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A312" s="11"/>
       <c r="B312" s="12"/>
       <c r="C312" s="12"/>
       <c r="D312" s="13"/>
-      <c r="E312" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C312))),C312,"")</f>
-        <v/>
-      </c>
+      <c r="E312" s="14"/>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A313" s="11"/>
       <c r="B313" s="12"/>
       <c r="C313" s="12"/>
       <c r="D313" s="13"/>
-      <c r="E313" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C313))),C313,"")</f>
-        <v/>
-      </c>
+      <c r="E313" s="14"/>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A314" s="11"/>
       <c r="B314" s="12"/>
       <c r="C314" s="12"/>
       <c r="D314" s="13"/>
-      <c r="E314" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C314))),C314,"")</f>
-        <v/>
-      </c>
+      <c r="E314" s="14"/>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A315" s="11"/>
       <c r="B315" s="12"/>
       <c r="C315" s="12"/>
       <c r="D315" s="13"/>
-      <c r="E315" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C315))),C315,"")</f>
-        <v/>
-      </c>
+      <c r="E315" s="14"/>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="11"/>
       <c r="B316" s="12"/>
       <c r="C316" s="12"/>
       <c r="D316" s="13"/>
-      <c r="E316" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C316))),C316,"")</f>
-        <v/>
-      </c>
+      <c r="E316" s="14"/>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A317" s="11"/>
       <c r="B317" s="12"/>
       <c r="C317" s="12"/>
       <c r="D317" s="13"/>
-      <c r="E317" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C317))),C317,"")</f>
-        <v/>
-      </c>
+      <c r="E317" s="14"/>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A318" s="11"/>
       <c r="B318" s="12"/>
       <c r="C318" s="12"/>
       <c r="D318" s="13"/>
-      <c r="E318" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C318))),C318,"")</f>
-        <v/>
-      </c>
+      <c r="E318" s="14"/>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A319" s="11"/>
       <c r="B319" s="12"/>
       <c r="C319" s="12"/>
       <c r="D319" s="13"/>
-      <c r="E319" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C319))),C319,"")</f>
-        <v/>
-      </c>
+      <c r="E319" s="14"/>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A320" s="11"/>
       <c r="B320" s="12"/>
       <c r="C320" s="12"/>
       <c r="D320" s="13"/>
-      <c r="E320" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C320))),C320,"")</f>
-        <v/>
-      </c>
+      <c r="E320" s="14"/>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A321" s="11"/>
       <c r="B321" s="12"/>
       <c r="C321" s="12"/>
       <c r="D321" s="13"/>
-      <c r="E321" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C321))),C321,"")</f>
-        <v/>
-      </c>
+      <c r="E321" s="14"/>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A322" s="11"/>
       <c r="B322" s="12"/>
       <c r="C322" s="12"/>
       <c r="D322" s="13"/>
-      <c r="E322" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C322))),C322,"")</f>
-        <v/>
-      </c>
+      <c r="E322" s="14"/>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A323" s="11"/>
       <c r="B323" s="12"/>
       <c r="C323" s="12"/>
       <c r="D323" s="13"/>
-      <c r="E323" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C323))),C323,"")</f>
-        <v/>
-      </c>
+      <c r="E323" s="14"/>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A324" s="11"/>
       <c r="B324" s="12"/>
       <c r="C324" s="12"/>
       <c r="D324" s="13"/>
-      <c r="E324" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C324))),C324,"")</f>
-        <v/>
-      </c>
+      <c r="E324" s="14"/>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A325" s="11"/>
       <c r="B325" s="12"/>
       <c r="C325" s="12"/>
       <c r="D325" s="13"/>
-      <c r="E325" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C325))),C325,"")</f>
-        <v/>
-      </c>
+      <c r="E325" s="14"/>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A326" s="11"/>
       <c r="B326" s="12"/>
       <c r="C326" s="12"/>
       <c r="D326" s="13"/>
-      <c r="E326" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C326))),C326,"")</f>
-        <v/>
-      </c>
+      <c r="E326" s="14"/>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A327" s="11"/>
       <c r="B327" s="12"/>
       <c r="C327" s="12"/>
       <c r="D327" s="13"/>
-      <c r="E327" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C327))),C327,"")</f>
-        <v/>
-      </c>
+      <c r="E327" s="14"/>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A328" s="11"/>
       <c r="B328" s="12"/>
       <c r="C328" s="12"/>
       <c r="D328" s="13"/>
-      <c r="E328" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C328))),C328,"")</f>
-        <v/>
-      </c>
+      <c r="E328" s="14"/>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="11"/>
       <c r="B329" s="12"/>
       <c r="C329" s="12"/>
       <c r="D329" s="13"/>
-      <c r="E329" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C329))),C329,"")</f>
-        <v/>
-      </c>
+      <c r="E329" s="14"/>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A330" s="11"/>
       <c r="B330" s="12"/>
       <c r="C330" s="12"/>
       <c r="D330" s="13"/>
-      <c r="E330" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C330))),C330,"")</f>
-        <v/>
-      </c>
+      <c r="E330" s="14"/>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A331" s="11"/>
       <c r="B331" s="12"/>
       <c r="C331" s="12"/>
       <c r="D331" s="13"/>
-      <c r="E331" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C331))),C331,"")</f>
-        <v/>
-      </c>
+      <c r="E331" s="14"/>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A332" s="11"/>
       <c r="B332" s="12"/>
       <c r="C332" s="12"/>
       <c r="D332" s="13"/>
-      <c r="E332" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C332))),C332,"")</f>
-        <v/>
-      </c>
+      <c r="E332" s="14"/>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A333" s="11"/>
       <c r="B333" s="12"/>
       <c r="C333" s="12"/>
       <c r="D333" s="13"/>
-      <c r="E333" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C333))),C333,"")</f>
-        <v/>
-      </c>
+      <c r="E333" s="14"/>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="11"/>
       <c r="B334" s="12"/>
       <c r="C334" s="12"/>
       <c r="D334" s="13"/>
-      <c r="E334" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C334))),C334,"")</f>
-        <v/>
-      </c>
+      <c r="E334" s="14"/>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A335" s="11"/>
       <c r="B335" s="12"/>
       <c r="C335" s="12"/>
       <c r="D335" s="13"/>
-      <c r="E335" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C335))),C335,"")</f>
-        <v/>
-      </c>
+      <c r="E335" s="14"/>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A336" s="11"/>
       <c r="B336" s="12"/>
       <c r="C336" s="12"/>
       <c r="D336" s="13"/>
-      <c r="E336" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C336))),C336,"")</f>
-        <v/>
-      </c>
+      <c r="E336" s="14"/>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A337" s="11"/>
       <c r="B337" s="12"/>
       <c r="C337" s="12"/>
       <c r="D337" s="13"/>
-      <c r="E337" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C337))),C337,"")</f>
-        <v/>
-      </c>
+      <c r="E337" s="14"/>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A338" s="11"/>
       <c r="B338" s="12"/>
       <c r="C338" s="12"/>
       <c r="D338" s="13"/>
-      <c r="E338" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C338))),C338,"")</f>
-        <v/>
-      </c>
+      <c r="E338" s="14"/>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A339" s="11"/>
       <c r="B339" s="12"/>
       <c r="C339" s="12"/>
       <c r="D339" s="13"/>
-      <c r="E339" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C339))),C339,"")</f>
-        <v/>
-      </c>
+      <c r="E339" s="14"/>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A340" s="11"/>
       <c r="B340" s="12"/>
       <c r="C340" s="12"/>
       <c r="D340" s="13"/>
-      <c r="E340" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C340))),C340,"")</f>
-        <v/>
-      </c>
+      <c r="E340" s="14"/>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A341" s="11"/>
       <c r="B341" s="12"/>
       <c r="C341" s="12"/>
       <c r="D341" s="13"/>
-      <c r="E341" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C341))),C341,"")</f>
-        <v/>
-      </c>
+      <c r="E341" s="14"/>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A342" s="11"/>
       <c r="B342" s="12"/>
       <c r="C342" s="12"/>
       <c r="D342" s="13"/>
-      <c r="E342" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C342))),C342,"")</f>
-        <v/>
-      </c>
+      <c r="E342" s="14"/>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A343" s="11"/>
       <c r="B343" s="12"/>
       <c r="C343" s="12"/>
       <c r="D343" s="13"/>
-      <c r="E343" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C343))),C343,"")</f>
-        <v/>
-      </c>
+      <c r="E343" s="14"/>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A344" s="11"/>
       <c r="B344" s="12"/>
       <c r="C344" s="12"/>
       <c r="D344" s="13"/>
-      <c r="E344" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C344))),C344,"")</f>
-        <v/>
-      </c>
+      <c r="E344" s="14"/>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A345" s="11"/>
       <c r="B345" s="12"/>
       <c r="C345" s="12"/>
       <c r="D345" s="13"/>
-      <c r="E345" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C345))),C345,"")</f>
-        <v/>
-      </c>
+      <c r="E345" s="14"/>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A346" s="11"/>
       <c r="B346" s="12"/>
       <c r="C346" s="12"/>
       <c r="D346" s="13"/>
-      <c r="E346" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C346))),C346,"")</f>
-        <v/>
-      </c>
+      <c r="E346" s="14"/>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A347" s="11"/>
       <c r="B347" s="12"/>
       <c r="C347" s="12"/>
       <c r="D347" s="13"/>
-      <c r="E347" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C347))),C347,"")</f>
-        <v/>
-      </c>
+      <c r="E347" s="14"/>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A348" s="11"/>
       <c r="B348" s="12"/>
       <c r="C348" s="12"/>
       <c r="D348" s="13"/>
-      <c r="E348" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C348))),C348,"")</f>
-        <v/>
-      </c>
+      <c r="E348" s="14"/>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A349" s="11"/>
       <c r="B349" s="12"/>
       <c r="C349" s="12"/>
       <c r="D349" s="13"/>
-      <c r="E349" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C349))),C349,"")</f>
-        <v/>
-      </c>
+      <c r="E349" s="14"/>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A350" s="11"/>
       <c r="B350" s="12"/>
       <c r="C350" s="12"/>
       <c r="D350" s="13"/>
-      <c r="E350" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C350))),C350,"")</f>
-        <v/>
-      </c>
+      <c r="E350" s="14"/>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A351" s="11"/>
       <c r="B351" s="12"/>
       <c r="C351" s="12"/>
       <c r="D351" s="13"/>
-      <c r="E351" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C351))),C351,"")</f>
-        <v/>
-      </c>
+      <c r="E351" s="14"/>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A352" s="11"/>
       <c r="B352" s="12"/>
       <c r="C352" s="12"/>
       <c r="D352" s="13"/>
-      <c r="E352" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C352))),C352,"")</f>
-        <v/>
-      </c>
+      <c r="E352" s="14"/>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A353" s="11"/>
       <c r="B353" s="12"/>
       <c r="C353" s="12"/>
       <c r="D353" s="13"/>
-      <c r="E353" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C353))),C353,"")</f>
-        <v/>
-      </c>
+      <c r="E353" s="14"/>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A354" s="11"/>
       <c r="B354" s="12"/>
       <c r="C354" s="12"/>
       <c r="D354" s="13"/>
-      <c r="E354" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C354))),C354,"")</f>
-        <v/>
-      </c>
+      <c r="E354" s="14"/>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A355" s="11"/>
       <c r="B355" s="12"/>
       <c r="C355" s="12"/>
       <c r="D355" s="13"/>
-      <c r="E355" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C355))),C355,"")</f>
-        <v/>
-      </c>
+      <c r="E355" s="14"/>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A356" s="11"/>
       <c r="B356" s="12"/>
       <c r="C356" s="12"/>
       <c r="D356" s="13"/>
-      <c r="E356" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C356))),C356,"")</f>
-        <v/>
-      </c>
+      <c r="E356" s="14"/>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A357" s="11"/>
       <c r="B357" s="12"/>
       <c r="C357" s="12"/>
       <c r="D357" s="13"/>
-      <c r="E357" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C357))),C357,"")</f>
-        <v/>
-      </c>
+      <c r="E357" s="14"/>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A358" s="11"/>
       <c r="B358" s="12"/>
       <c r="C358" s="12"/>
       <c r="D358" s="13"/>
-      <c r="E358" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C358))),C358,"")</f>
-        <v/>
-      </c>
+      <c r="E358" s="14"/>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A359" s="11"/>
       <c r="B359" s="12"/>
       <c r="C359" s="12"/>
       <c r="D359" s="13"/>
-      <c r="E359" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C359))),C359,"")</f>
-        <v/>
-      </c>
+      <c r="E359" s="14"/>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A360" s="11"/>
       <c r="B360" s="12"/>
       <c r="C360" s="12"/>
       <c r="D360" s="13"/>
-      <c r="E360" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C360))),C360,"")</f>
-        <v/>
-      </c>
+      <c r="E360" s="14"/>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A361" s="11"/>
       <c r="B361" s="12"/>
       <c r="C361" s="12"/>
       <c r="D361" s="13"/>
-      <c r="E361" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C361))),C361,"")</f>
-        <v/>
-      </c>
+      <c r="E361" s="14"/>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A362" s="11"/>
       <c r="B362" s="12"/>
       <c r="C362" s="12"/>
       <c r="D362" s="13"/>
-      <c r="E362" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C362))),C362,"")</f>
-        <v/>
-      </c>
+      <c r="E362" s="14"/>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A363" s="11"/>
       <c r="B363" s="12"/>
       <c r="C363" s="12"/>
       <c r="D363" s="13"/>
-      <c r="E363" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C363))),C363,"")</f>
-        <v/>
-      </c>
+      <c r="E363" s="14"/>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A364" s="11"/>
       <c r="B364" s="12"/>
       <c r="C364" s="12"/>
       <c r="D364" s="13"/>
-      <c r="E364" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C364))),C364,"")</f>
-        <v/>
-      </c>
+      <c r="E364" s="14"/>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A365" s="11"/>
       <c r="B365" s="12"/>
       <c r="C365" s="12"/>
       <c r="D365" s="13"/>
-      <c r="E365" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C365))),C365,"")</f>
-        <v/>
-      </c>
+      <c r="E365" s="14"/>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A366" s="11"/>
       <c r="B366" s="12"/>
       <c r="C366" s="12"/>
       <c r="D366" s="13"/>
-      <c r="E366" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C366))),C366,"")</f>
-        <v/>
-      </c>
+      <c r="E366" s="14"/>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A367" s="11"/>
       <c r="B367" s="12"/>
       <c r="C367" s="12"/>
       <c r="D367" s="13"/>
-      <c r="E367" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C367))),C367,"")</f>
-        <v/>
-      </c>
+      <c r="E367" s="14"/>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A368" s="11"/>
       <c r="B368" s="12"/>
       <c r="C368" s="12"/>
       <c r="D368" s="13"/>
-      <c r="E368" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C368))),C368,"")</f>
-        <v/>
-      </c>
+      <c r="E368" s="14"/>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A369" s="11"/>
       <c r="B369" s="12"/>
       <c r="C369" s="12"/>
       <c r="D369" s="13"/>
-      <c r="E369" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C369))),C369,"")</f>
-        <v/>
-      </c>
+      <c r="E369" s="14"/>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A370" s="11"/>
       <c r="B370" s="12"/>
       <c r="C370" s="12"/>
       <c r="D370" s="13"/>
-      <c r="E370" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C370))),C370,"")</f>
-        <v/>
-      </c>
+      <c r="E370" s="14"/>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A371" s="11"/>
       <c r="B371" s="12"/>
       <c r="C371" s="12"/>
       <c r="D371" s="13"/>
-      <c r="E371" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C371))),C371,"")</f>
-        <v/>
-      </c>
+      <c r="E371" s="14"/>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A372" s="11"/>
       <c r="B372" s="12"/>
       <c r="C372" s="12"/>
       <c r="D372" s="13"/>
-      <c r="E372" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C372))),C372,"")</f>
-        <v/>
-      </c>
+      <c r="E372" s="14"/>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A373" s="11"/>
       <c r="B373" s="12"/>
       <c r="C373" s="12"/>
       <c r="D373" s="13"/>
-      <c r="E373" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C373))),C373,"")</f>
-        <v/>
-      </c>
+      <c r="E373" s="14"/>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A374" s="11"/>
       <c r="B374" s="12"/>
       <c r="C374" s="12"/>
       <c r="D374" s="13"/>
-      <c r="E374" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C374))),C374,"")</f>
-        <v/>
-      </c>
+      <c r="E374" s="14"/>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A375" s="11"/>
       <c r="B375" s="12"/>
       <c r="C375" s="12"/>
       <c r="D375" s="13"/>
-      <c r="E375" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C375))),C375,"")</f>
-        <v/>
-      </c>
+      <c r="E375" s="14"/>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A376" s="11"/>
       <c r="B376" s="12"/>
       <c r="C376" s="12"/>
       <c r="D376" s="13"/>
-      <c r="E376" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C376))),C376,"")</f>
-        <v/>
-      </c>
+      <c r="E376" s="14"/>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A377" s="11"/>
       <c r="B377" s="12"/>
       <c r="C377" s="12"/>
       <c r="D377" s="13"/>
-      <c r="E377" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C377))),C377,"")</f>
-        <v/>
-      </c>
+      <c r="E377" s="14"/>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A378" s="11"/>
       <c r="B378" s="12"/>
       <c r="C378" s="12"/>
       <c r="D378" s="13"/>
-      <c r="E378" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C378))),C378,"")</f>
-        <v/>
-      </c>
+      <c r="E378" s="14"/>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A379" s="11"/>
       <c r="B379" s="12"/>
       <c r="C379" s="12"/>
       <c r="D379" s="13"/>
-      <c r="E379" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C379))),C379,"")</f>
-        <v/>
-      </c>
+      <c r="E379" s="14"/>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A380" s="11"/>
       <c r="B380" s="12"/>
       <c r="C380" s="12"/>
       <c r="D380" s="13"/>
-      <c r="E380" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C380))),C380,"")</f>
-        <v/>
-      </c>
+      <c r="E380" s="14"/>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A381" s="11"/>
       <c r="B381" s="12"/>
       <c r="C381" s="12"/>
       <c r="D381" s="13"/>
-      <c r="E381" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C381))),C381,"")</f>
-        <v/>
-      </c>
+      <c r="E381" s="14"/>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A382" s="11"/>
       <c r="B382" s="12"/>
       <c r="C382" s="12"/>
       <c r="D382" s="13"/>
-      <c r="E382" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C382))),C382,"")</f>
-        <v/>
-      </c>
+      <c r="E382" s="14"/>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A383" s="11"/>
       <c r="B383" s="12"/>
       <c r="C383" s="12"/>
       <c r="D383" s="13"/>
-      <c r="E383" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C383))),C383,"")</f>
-        <v/>
-      </c>
+      <c r="E383" s="14"/>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A384" s="11"/>
       <c r="B384" s="12"/>
       <c r="C384" s="12"/>
       <c r="D384" s="13"/>
-      <c r="E384" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C384))),C384,"")</f>
-        <v/>
-      </c>
+      <c r="E384" s="14"/>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A385" s="11"/>
       <c r="B385" s="12"/>
       <c r="C385" s="12"/>
       <c r="D385" s="13"/>
-      <c r="E385" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C385))),C385,"")</f>
-        <v/>
-      </c>
+      <c r="E385" s="14"/>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A386" s="11"/>
       <c r="B386" s="12"/>
       <c r="C386" s="12"/>
       <c r="D386" s="13"/>
-      <c r="E386" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C386))),C386,"")</f>
-        <v/>
-      </c>
+      <c r="E386" s="14"/>
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A387" s="11"/>
       <c r="B387" s="12"/>
       <c r="C387" s="12"/>
       <c r="D387" s="13"/>
-      <c r="E387" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C387))),C387,"")</f>
-        <v/>
-      </c>
+      <c r="E387" s="14"/>
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A388" s="11"/>
       <c r="B388" s="12"/>
       <c r="C388" s="12"/>
       <c r="D388" s="13"/>
-      <c r="E388" s="14" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C388))),C388,"")</f>
-        <v/>
-      </c>
+      <c r="E388" s="14"/>
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A389" s="15"/>
       <c r="B389" s="16"/>
       <c r="C389" s="16"/>
       <c r="D389" s="17"/>
-      <c r="E389" s="18" t="str">
-        <f aca="false">IF(AND(E$2="Yes",NOT(ISBLANK($C389))),C389,"")</f>
-        <v/>
-      </c>
+      <c r="E389" s="18"/>
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6132,7 +4979,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.33"/>
   </cols>
@@ -7072,7 +5919,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.5"/>

</xml_diff>